<commit_message>
Lots of changes to rmd Creating a new model in model-making for low quality. Adding features for tables such as dagger and asterisks signs based on matching_age and matching_education. NB - asterisks are complex as they are also markdown in themselves! Figuring out how make columns md- operable with as_flextable and column_md Fixing tweak in quality plot order
</commit_message>
<xml_diff>
--- a/Data_SR.xlsx
+++ b/Data_SR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2509920f_student_gla_ac_uk/Documents/DClin/Deliverables/Systematic Review/Writeup/DCLIN_SR_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4787" documentId="8_{7F86DA56-8D65-4C4F-B68E-F6A80F78D27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DAE71CF-99ED-434B-AA0F-CD83BC4A2989}"/>
+  <xr:revisionPtr revIDLastSave="4790" documentId="8_{7F86DA56-8D65-4C4F-B68E-F6A80F78D27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4AF939B-2D30-48F9-87FC-8BCBBB3008B9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="700">
   <si>
     <t>MMSE</t>
   </si>
@@ -2306,9 +2306,6 @@
   </si>
   <si>
     <t>significant</t>
-  </si>
-  <si>
-    <t>ACE-R</t>
   </si>
   <si>
     <t>III</t>
@@ -3026,10 +3023,10 @@
   <dimension ref="A1:DX64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="U43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3155,7 +3152,7 @@
         <v>489</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="V1" s="6" t="s">
         <v>375</v>
@@ -3412,10 +3409,10 @@
         <v>46</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="13" t="s">
@@ -3449,7 +3446,7 @@
         <v>491</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V2" s="19">
         <v>100</v>
@@ -3642,10 +3639,10 @@
         <v>48</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13" t="s">
@@ -3676,10 +3673,10 @@
         <v>476</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V3" s="13">
         <v>39</v>
@@ -3886,10 +3883,10 @@
         <v>57</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="19" t="s">
@@ -3923,7 +3920,7 @@
         <v>58</v>
       </c>
       <c r="U4" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V4" s="13">
         <v>30</v>
@@ -4107,7 +4104,7 @@
         <v>536</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13" t="s">
@@ -4141,7 +4138,7 @@
         <v>490</v>
       </c>
       <c r="U5" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V5" s="13">
         <v>16</v>
@@ -4321,7 +4318,7 @@
         <v>536</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13" t="s">
@@ -4355,7 +4352,7 @@
         <v>58</v>
       </c>
       <c r="U6" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V6" s="13">
         <v>18</v>
@@ -4556,7 +4553,7 @@
         <v>546</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>542</v>
@@ -4593,7 +4590,7 @@
         <v>490</v>
       </c>
       <c r="U7" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V7" s="13">
         <v>8</v>
@@ -4792,10 +4789,10 @@
         <v>103</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13" t="s">
@@ -4829,7 +4826,7 @@
         <v>492</v>
       </c>
       <c r="U8" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V8" s="13">
         <v>40</v>
@@ -5055,7 +5052,7 @@
         <v>536</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>677</v>
@@ -5091,7 +5088,7 @@
         <v>491</v>
       </c>
       <c r="U9" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V9" s="13">
         <v>16</v>
@@ -5297,7 +5294,7 @@
         <v>536</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>677</v>
@@ -5333,7 +5330,7 @@
         <v>491</v>
       </c>
       <c r="U10" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V10" s="13">
         <v>16</v>
@@ -5532,10 +5529,10 @@
         <v>459</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13" t="s">
@@ -5565,7 +5562,7 @@
         <v>493</v>
       </c>
       <c r="U11" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V11" s="13">
         <v>45</v>
@@ -5750,10 +5747,10 @@
         <v>138</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="13" t="s">
@@ -5783,7 +5780,7 @@
         <v>490</v>
       </c>
       <c r="U12" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V12" s="13">
         <v>31</v>
@@ -5967,7 +5964,7 @@
         <v>115</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13" t="s">
@@ -6001,7 +5998,7 @@
         <v>490</v>
       </c>
       <c r="U13" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V13" s="13">
         <v>23</v>
@@ -6188,10 +6185,10 @@
         <v>145</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J14" s="13"/>
       <c r="K14" s="13" t="s">
@@ -6225,7 +6222,7 @@
         <v>493</v>
       </c>
       <c r="U14" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V14" s="13">
         <v>96</v>
@@ -6400,10 +6397,10 @@
         <v>149</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13" t="s">
@@ -6433,7 +6430,7 @@
         <v>153</v>
       </c>
       <c r="U15" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V15" s="13">
         <v>30</v>
@@ -6601,7 +6598,7 @@
         <v>115</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="13" t="s">
@@ -6635,7 +6632,7 @@
         <v>58</v>
       </c>
       <c r="U16" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V16" s="13">
         <v>10</v>
@@ -6841,7 +6838,7 @@
         <v>115</v>
       </c>
       <c r="I17" s="35" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13" t="s">
@@ -6875,7 +6872,7 @@
         <v>494</v>
       </c>
       <c r="U17" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V17" s="13">
         <v>10</v>
@@ -7081,7 +7078,7 @@
         <v>537</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13" t="s">
@@ -7115,7 +7112,7 @@
         <v>495</v>
       </c>
       <c r="U18" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V18" s="13">
         <v>12</v>
@@ -7315,7 +7312,7 @@
         <v>115</v>
       </c>
       <c r="I19" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13" t="s">
@@ -7349,7 +7346,7 @@
         <v>496</v>
       </c>
       <c r="U19" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V19" s="13">
         <v>10</v>
@@ -7534,10 +7531,10 @@
         <v>175</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13" t="s">
@@ -7562,16 +7559,16 @@
         <v>34</v>
       </c>
       <c r="R20" s="13" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="S20" s="19" t="s">
         <v>173</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U20" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V20" s="13">
         <v>45</v>
@@ -7744,10 +7741,10 @@
         <v>181</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13" t="s">
@@ -7781,7 +7778,7 @@
         <v>493</v>
       </c>
       <c r="U21" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V21" s="13">
         <v>37</v>
@@ -7979,7 +7976,7 @@
         <v>536</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J22" s="13" t="s">
         <v>349</v>
@@ -7988,7 +7985,7 @@
         <v>60</v>
       </c>
       <c r="L22" s="19" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="M22" s="13">
         <v>28</v>
@@ -8009,13 +8006,13 @@
         <v>118</v>
       </c>
       <c r="S22" s="19" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="T22" s="19" t="s">
         <v>493</v>
       </c>
       <c r="U22" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V22" s="13">
         <v>38</v>
@@ -8033,10 +8030,10 @@
         <v>25</v>
       </c>
       <c r="AA22" s="13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="AB22" s="13" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AC22" s="13" t="s">
         <v>42</v>
@@ -8218,10 +8215,10 @@
         <v>191</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J23" s="13"/>
       <c r="K23" s="13" t="s">
@@ -8246,16 +8243,16 @@
         <v>43</v>
       </c>
       <c r="R23" s="13" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="S23" s="19" t="s">
         <v>193</v>
       </c>
       <c r="T23" s="19" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U23" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V23" s="13">
         <v>476</v>
@@ -8464,16 +8461,16 @@
         <v>16</v>
       </c>
       <c r="R24" s="13" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="S24" s="19" t="s">
         <v>201</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U24" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V24" s="13">
         <v>85</v>
@@ -8682,10 +8679,10 @@
         <v>203</v>
       </c>
       <c r="T25" s="19" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U25" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V25" s="13">
         <v>3250</v>
@@ -8869,7 +8866,7 @@
         <v>115</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J26" s="13"/>
       <c r="K26" s="13" t="s">
@@ -8903,7 +8900,7 @@
         <v>493</v>
       </c>
       <c r="U26" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V26" s="13">
         <v>30</v>
@@ -9121,7 +9118,7 @@
         <v>115</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J27" s="13"/>
       <c r="K27" s="13" t="s">
@@ -9155,7 +9152,7 @@
         <v>493</v>
       </c>
       <c r="U27" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V27" s="13">
         <v>30</v>
@@ -9375,7 +9372,7 @@
         <v>115</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J28" s="13"/>
       <c r="K28" s="13" t="s">
@@ -9409,7 +9406,7 @@
         <v>491</v>
       </c>
       <c r="U28" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V28" s="13">
         <v>44</v>
@@ -9588,10 +9585,10 @@
         <v>355</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>358</v>
@@ -9627,7 +9624,7 @@
         <v>493</v>
       </c>
       <c r="U29" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V29" s="13">
         <v>20</v>
@@ -9828,7 +9825,7 @@
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>542</v>
@@ -9867,7 +9864,7 @@
         <v>497</v>
       </c>
       <c r="U30" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V30" s="13">
         <v>104</v>
@@ -10076,7 +10073,7 @@
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>542</v>
@@ -10115,7 +10112,7 @@
         <v>490</v>
       </c>
       <c r="U31" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V31" s="13">
         <v>99</v>
@@ -10324,7 +10321,7 @@
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I32" s="13" t="s">
         <v>542</v>
@@ -10363,7 +10360,7 @@
         <v>58</v>
       </c>
       <c r="U32" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V32" s="13">
         <v>51</v>
@@ -10572,7 +10569,7 @@
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I33" s="13" t="s">
         <v>542</v>
@@ -10611,7 +10608,7 @@
         <v>497</v>
       </c>
       <c r="U33" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V33" s="13">
         <v>104</v>
@@ -10820,7 +10817,7 @@
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I34" s="13" t="s">
         <v>542</v>
@@ -10859,7 +10856,7 @@
         <v>490</v>
       </c>
       <c r="U34" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V34" s="13">
         <v>99</v>
@@ -11068,7 +11065,7 @@
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I35" s="13" t="s">
         <v>542</v>
@@ -11107,7 +11104,7 @@
         <v>58</v>
       </c>
       <c r="U35" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V35" s="13">
         <v>51</v>
@@ -11318,10 +11315,10 @@
         <v>247</v>
       </c>
       <c r="H36" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J36" s="13"/>
       <c r="K36" s="13" t="s">
@@ -11355,7 +11352,7 @@
         <v>493</v>
       </c>
       <c r="U36" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V36" s="13">
         <v>60</v>
@@ -11554,10 +11551,10 @@
         <v>251</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J37" s="13"/>
       <c r="K37" s="13" t="s">
@@ -11588,10 +11585,10 @@
         <v>250</v>
       </c>
       <c r="T37" s="19" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="U37" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V37" s="13">
         <v>34</v>
@@ -11782,10 +11779,10 @@
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J38" s="13"/>
       <c r="K38" s="13" t="s">
@@ -11813,13 +11810,13 @@
         <v>118</v>
       </c>
       <c r="S38" s="19" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="T38" s="19" t="s">
         <v>493</v>
       </c>
       <c r="U38" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V38" s="13">
         <v>30</v>
@@ -12012,10 +12009,10 @@
         <v>264</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J39" s="13"/>
       <c r="K39" s="13" t="s">
@@ -12047,7 +12044,7 @@
         <v>491</v>
       </c>
       <c r="U39" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V39" s="13">
         <v>51</v>
@@ -12233,7 +12230,7 @@
         <v>537</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J40" s="13"/>
       <c r="K40" s="13" t="s">
@@ -12267,7 +12264,7 @@
         <v>490</v>
       </c>
       <c r="U40" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V40" s="13">
         <v>30</v>
@@ -12457,7 +12454,7 @@
         <v>115</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J41" s="13"/>
       <c r="K41" s="13" t="s">
@@ -12491,7 +12488,7 @@
         <v>498</v>
       </c>
       <c r="U41" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V41" s="13">
         <v>10</v>
@@ -12684,10 +12681,10 @@
         <v>282</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J42" s="13"/>
       <c r="K42" s="13" t="s">
@@ -12721,7 +12718,7 @@
         <v>153</v>
       </c>
       <c r="U42" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V42" s="13">
         <v>12</v>
@@ -12910,10 +12907,10 @@
         <v>288</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J43" s="13"/>
       <c r="K43" s="13" t="s">
@@ -12942,10 +12939,10 @@
         <v>287</v>
       </c>
       <c r="T43" s="19" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U43" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V43" s="13">
         <v>44</v>
@@ -12963,7 +12960,7 @@
         <v>36</v>
       </c>
       <c r="AA43" s="13" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="AB43" s="13" t="s">
         <v>499</v>
@@ -13138,10 +13135,10 @@
         <v>295</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J44" s="13"/>
       <c r="K44" s="13" t="s">
@@ -13170,10 +13167,10 @@
         <v>287</v>
       </c>
       <c r="T44" s="19" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U44" s="19" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V44" s="13">
         <v>44</v>
@@ -13191,10 +13188,10 @@
         <v>39</v>
       </c>
       <c r="AA44" s="13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="AB44" s="13" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="AC44" s="13" t="s">
         <v>42</v>
@@ -13405,7 +13402,7 @@
         <v>58</v>
       </c>
       <c r="U45" s="13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V45" s="13">
         <v>30</v>
@@ -13586,10 +13583,10 @@
         <v>305</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J46" s="13"/>
       <c r="K46" s="13" t="s">
@@ -13623,7 +13620,7 @@
         <v>491</v>
       </c>
       <c r="U46" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V46" s="13">
         <v>11</v>
@@ -13837,7 +13834,7 @@
         <v>536</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J47" s="13" t="s">
         <v>314</v>
@@ -13867,13 +13864,13 @@
         <v>58</v>
       </c>
       <c r="S47" s="13" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="T47" s="13" t="s">
         <v>58</v>
       </c>
       <c r="U47" s="13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V47" s="13">
         <v>35</v>
@@ -14071,7 +14068,7 @@
         <v>115</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J48" s="13"/>
       <c r="K48" s="13" t="s">
@@ -14103,7 +14100,7 @@
         <v>491</v>
       </c>
       <c r="U48" s="30" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V48" s="13">
         <v>17</v>
@@ -14275,7 +14272,7 @@
         <v>115</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J49" s="13"/>
       <c r="K49" s="13" t="s">
@@ -14307,7 +14304,7 @@
         <v>491</v>
       </c>
       <c r="U49" s="30" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V49" s="13">
         <v>17</v>
@@ -14474,10 +14471,10 @@
       </c>
       <c r="G50" s="13"/>
       <c r="H50" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J50" s="13"/>
       <c r="K50" s="13" t="s">
@@ -14511,7 +14508,7 @@
         <v>497</v>
       </c>
       <c r="U50" s="13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V50" s="13">
         <v>36</v>
@@ -14690,10 +14687,10 @@
         <v>99</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J51" s="17"/>
       <c r="K51" s="14" t="s">
@@ -14727,7 +14724,7 @@
         <v>490</v>
       </c>
       <c r="U51" s="14" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V51" s="14">
         <v>163</v>
@@ -14924,10 +14921,10 @@
         <v>512</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J52" s="17" t="s">
         <v>520</v>
@@ -14959,7 +14956,7 @@
         <v>491</v>
       </c>
       <c r="U52" s="14" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V52" s="14">
         <v>88</v>
@@ -15170,10 +15167,10 @@
         <v>337</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J53" s="13"/>
       <c r="K53" s="13" t="s">
@@ -15207,7 +15204,7 @@
         <v>58</v>
       </c>
       <c r="U53" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V53" s="13">
         <v>50</v>
@@ -15376,10 +15373,10 @@
       </c>
       <c r="G54" s="57"/>
       <c r="H54" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J54" s="57"/>
       <c r="K54" s="13" t="s">
@@ -15413,7 +15410,7 @@
         <v>493</v>
       </c>
       <c r="U54" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V54" s="57">
         <v>29</v>
@@ -15602,10 +15599,10 @@
         <v>629</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J55" s="57"/>
       <c r="K55" s="13" t="s">
@@ -15639,7 +15636,7 @@
         <v>493</v>
       </c>
       <c r="U55" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V55" s="57">
         <v>20</v>
@@ -15816,10 +15813,10 @@
         <v>640</v>
       </c>
       <c r="H56" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I56" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J56" s="40" t="s">
         <v>637</v>
@@ -15855,7 +15852,7 @@
         <v>493</v>
       </c>
       <c r="U56" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V56" s="40">
         <v>210</v>
@@ -15968,10 +15965,10 @@
         <v>640</v>
       </c>
       <c r="H57" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I57" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J57" s="40" t="s">
         <v>637</v>
@@ -16007,7 +16004,7 @@
         <v>493</v>
       </c>
       <c r="U57" s="19" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V57" s="40">
         <v>210</v>
@@ -16120,10 +16117,10 @@
         <v>645</v>
       </c>
       <c r="H58" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I58" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="K58" s="13" t="s">
         <v>60</v>
@@ -16156,7 +16153,7 @@
         <v>493</v>
       </c>
       <c r="U58" s="56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V58" s="40">
         <v>67</v>
@@ -16263,10 +16260,10 @@
         <v>645</v>
       </c>
       <c r="H59" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I59" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="K59" s="13" t="s">
         <v>60</v>
@@ -16299,7 +16296,7 @@
         <v>493</v>
       </c>
       <c r="U59" s="56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V59" s="40">
         <v>35</v>
@@ -16406,10 +16403,10 @@
         <v>652</v>
       </c>
       <c r="H60" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I60" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="K60" s="13" t="s">
         <v>60</v>
@@ -16442,7 +16439,7 @@
         <v>493</v>
       </c>
       <c r="U60" s="56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V60" s="40">
         <v>45</v>
@@ -16553,10 +16550,10 @@
         <v>622</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I61" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J61" s="40" t="s">
         <v>623</v>
@@ -16592,7 +16589,7 @@
         <v>493</v>
       </c>
       <c r="U61" s="56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V61" s="40">
         <v>55</v>
@@ -16691,7 +16688,7 @@
         <v>115</v>
       </c>
       <c r="I62" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="K62" s="13" t="s">
         <v>60</v>
@@ -16724,7 +16721,7 @@
         <v>493</v>
       </c>
       <c r="U62" s="56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V62" s="40">
         <v>30</v>
@@ -16795,10 +16792,10 @@
         <v>527</v>
       </c>
       <c r="H63" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I63" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J63" s="59"/>
       <c r="K63" s="13" t="s">
@@ -16832,7 +16829,7 @@
         <v>153</v>
       </c>
       <c r="U63" s="35" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V63" s="35">
         <v>19</v>
@@ -17026,7 +17023,7 @@
         <v>536</v>
       </c>
       <c r="I64" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J64" s="35" t="s">
         <v>487</v>
@@ -17062,7 +17059,7 @@
         <v>58</v>
       </c>
       <c r="U64" s="56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V64" s="35">
         <v>459</v>

</xml_diff>